<commit_message>
some changes in utils
</commit_message>
<xml_diff>
--- a/img/tables.xlsx
+++ b/img/tables.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhorm\Documents\Master_IA\2022\NLU\P2_repo\depencendy_parsing\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F5588068-3BDB-43DA-98FC-1C32FF71DBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4B8362-DF21-494B-BE03-28523F53790F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="df_res_optimizers_models2" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -43,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
   <si>
     <t>arquitecture</t>
   </si>
@@ -130,12 +143,153 @@
   </si>
   <si>
     <t>String</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Action Accuracy</t>
+  </si>
+  <si>
+    <t>Deprel Accuracy</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>74.87</t>
+  </si>
+  <si>
+    <t>62.71</t>
+  </si>
+  <si>
+    <t>72.20</t>
+  </si>
+  <si>
+    <t>63.92</t>
+  </si>
+  <si>
+    <t>72.80</t>
+  </si>
+  <si>
+    <t>64.16</t>
+  </si>
+  <si>
+    <t>75.13</t>
+  </si>
+  <si>
+    <t>66.28</t>
+  </si>
+  <si>
+    <t>79.08</t>
+  </si>
+  <si>
+    <t>66.73</t>
+  </si>
+  <si>
+    <t>75.53</t>
+  </si>
+  <si>
+    <t>60.01</t>
+  </si>
+  <si>
+    <t>72.04</t>
+  </si>
+  <si>
+    <t>59.64</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>Optimizer</t>
+  </si>
+  <si>
+    <t>Optimizer and Learning rate</t>
+  </si>
+  <si>
+    <t>Early Stop and Patience</t>
+  </si>
+  <si>
+    <t>Embedding sizes</t>
+  </si>
+  <si>
+    <t>Stack and Buffer sizes</t>
+  </si>
+  <si>
+    <t>Batch sizes</t>
+  </si>
+  <si>
+    <t>A. Accuracy</t>
+  </si>
+  <si>
+    <t>D. Accuracy</t>
+  </si>
+  <si>
+    <t>A. Loss</t>
+  </si>
+  <si>
+    <t>D. Loss</t>
+  </si>
+  <si>
+    <t>(200, 350)</t>
+  </si>
+  <si>
+    <t>output_deprel_accuracy</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Buffer</t>
+  </si>
+  <si>
+    <t>Patience</t>
+  </si>
+  <si>
+    <t>Time (s)</t>
+  </si>
+  <si>
+    <t>Embedding</t>
+  </si>
+  <si>
+    <t>Batch size</t>
+  </si>
+  <si>
+    <t>Learning rate</t>
+  </si>
+  <si>
+    <t>Early Stop</t>
+  </si>
+  <si>
+    <t>SGD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="172" formatCode="0.000"/>
+    <numFmt numFmtId="173" formatCode="0.0"/>
+  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -286,7 +440,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -478,8 +632,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -609,6 +775,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -655,15 +847,49 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1019,11 +1245,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,7 +1881,7 @@
         <f t="shared" si="0"/>
         <v>1024</v>
       </c>
-      <c r="I24" s="5"/>
+      <c r="I24" s="2"/>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C25">
@@ -1675,98 +1901,550 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B3:Q36"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="11.42578125" style="4"/>
+    <col min="5" max="5" width="7.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="17" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="4"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="F8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="F9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="F10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+      <c r="F11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="F12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="F13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0.90107429027557295</v>
+      </c>
+      <c r="H19" s="8">
+        <v>0.87854373455047596</v>
+      </c>
+      <c r="I19" s="9">
+        <v>0.255371153354644</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0.38322558999061501</v>
+      </c>
+    </row>
+    <row r="20" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F20" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0.902715623378753</v>
+      </c>
+      <c r="H20" s="8">
+        <v>0.87093406915664595</v>
+      </c>
+      <c r="I20" s="9">
+        <v>0.25959685444831798</v>
+      </c>
+      <c r="J20" s="9">
+        <v>0.39582976698875399</v>
+      </c>
+    </row>
+    <row r="21" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F21" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0.90196955204009999</v>
+      </c>
+      <c r="H21" s="8">
+        <v>0.88167709112167303</v>
+      </c>
+      <c r="I21" s="9">
+        <v>0.25990459322929299</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0.37431794404983498</v>
+      </c>
+    </row>
+    <row r="22" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0.90316325426101596</v>
+      </c>
+      <c r="H22" s="8">
+        <v>0.88287079334259</v>
+      </c>
+      <c r="I22" s="9">
+        <v>0.26155197620391801</v>
+      </c>
+      <c r="J22" s="9">
+        <v>0.39369285106658902</v>
+      </c>
+    </row>
+    <row r="23" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F23" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0.90316325426101596</v>
+      </c>
+      <c r="H23" s="8">
+        <v>0.87615638971328702</v>
+      </c>
+      <c r="I23" s="9">
+        <v>0.25941577553749001</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0.38542091846465998</v>
+      </c>
+    </row>
+    <row r="27" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F27" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="L27" s="15"/>
+    </row>
+    <row r="28" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F28" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="13">
+        <v>512</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="I28" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="K28" s="13">
+        <v>17</v>
+      </c>
+      <c r="L28" s="13"/>
+      <c r="P28" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q28" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F29" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="P29" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q29" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F30" s="13">
+        <v>2</v>
+      </c>
+      <c r="G30" s="13">
+        <v>3</v>
+      </c>
+      <c r="H30" s="10">
+        <v>0.902715623378753</v>
+      </c>
+      <c r="I30" s="10">
+        <v>0.87541031837463301</v>
+      </c>
+      <c r="J30" s="9">
+        <v>0.269791960716247</v>
+      </c>
+      <c r="K30" s="9">
+        <v>0.39209842681884699</v>
+      </c>
+      <c r="L30" s="9">
+        <v>35.8665449619293</v>
+      </c>
+      <c r="P30" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q30" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F31" s="13">
+        <v>3</v>
+      </c>
+      <c r="G31" s="13">
+        <v>3</v>
+      </c>
+      <c r="H31" s="10">
+        <v>0.90226799249649003</v>
+      </c>
+      <c r="I31" s="10">
+        <v>0.87436586618423395</v>
+      </c>
+      <c r="J31" s="9">
+        <v>0.25716364383697499</v>
+      </c>
+      <c r="K31" s="9">
+        <v>0.39230364561080899</v>
+      </c>
+      <c r="L31" s="9">
+        <v>37.489367723464902</v>
+      </c>
+      <c r="P31" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q31" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F32" s="13">
+        <v>5</v>
+      </c>
+      <c r="G32" s="13">
+        <v>5</v>
+      </c>
+      <c r="H32" s="10">
+        <v>0.90062665939330999</v>
+      </c>
+      <c r="I32" s="10">
+        <v>0.874664306640625</v>
+      </c>
+      <c r="J32" s="9">
+        <v>0.25856274366378701</v>
+      </c>
+      <c r="K32" s="9">
+        <v>0.39108017086982699</v>
+      </c>
+      <c r="L32" s="9">
+        <v>45.091784715652402</v>
+      </c>
+      <c r="P32" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q32" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F33" s="13">
+        <v>6</v>
+      </c>
+      <c r="G33" s="13">
+        <v>6</v>
+      </c>
+      <c r="H33" s="10">
+        <v>0.90569978952407804</v>
+      </c>
+      <c r="I33" s="10">
+        <v>0.87003880739212003</v>
+      </c>
+      <c r="J33" s="9">
+        <v>0.25609907507896401</v>
+      </c>
+      <c r="K33" s="9">
+        <v>0.41229891777038502</v>
+      </c>
+      <c r="L33" s="9">
+        <v>48.572444677352898</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q33" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F34" s="13">
+        <v>8</v>
+      </c>
+      <c r="G34" s="13">
+        <v>8</v>
+      </c>
+      <c r="H34" s="10">
+        <v>0.90077590942382801</v>
+      </c>
+      <c r="I34" s="10">
+        <v>0.87764847278594904</v>
+      </c>
+      <c r="J34" s="9">
+        <v>0.26552155613899198</v>
+      </c>
+      <c r="K34" s="9">
+        <v>0.39451083540916398</v>
+      </c>
+      <c r="L34" s="9">
+        <v>56.144419193267801</v>
+      </c>
+    </row>
+    <row r="35" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F35" s="13">
+        <v>10</v>
+      </c>
+      <c r="G35" s="13">
+        <v>10</v>
+      </c>
+      <c r="H35" s="10">
+        <v>0.90405851602554299</v>
+      </c>
+      <c r="I35" s="10">
+        <v>0.86332440376281705</v>
+      </c>
+      <c r="J35" s="9">
+        <v>0.26171118021011303</v>
+      </c>
+      <c r="K35" s="9">
+        <v>0.41729778051376298</v>
+      </c>
+      <c r="L35" s="9">
+        <v>64.464055538177405</v>
+      </c>
+    </row>
+    <row r="36" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F36" s="13">
+        <v>12</v>
+      </c>
+      <c r="G36" s="13">
+        <v>12</v>
+      </c>
+      <c r="H36" s="10">
+        <v>0.89913457632064797</v>
+      </c>
+      <c r="I36" s="10">
+        <v>0.87093406915664595</v>
+      </c>
+      <c r="J36" s="9">
+        <v>0.26804059743881198</v>
+      </c>
+      <c r="K36" s="9">
+        <v>0.39901617169380099</v>
+      </c>
+      <c r="L36" s="9">
+        <v>71.957367181777897</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K27:L27"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>